<commit_message>
Need to be Upgraded
</commit_message>
<xml_diff>
--- a/Output/Candidates.xlsx
+++ b/Output/Candidates.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <x:si>
     <x:t>Name</x:t>
   </x:si>
@@ -31,6 +31,9 @@
     <x:t>Mobile_Phone</x:t>
   </x:si>
   <x:si>
+    <x:t>Sender</x:t>
+  </x:si>
+  <x:si>
     <x:t>FELE</x:t>
   </x:si>
   <x:si>
@@ -44,6 +47,9 @@
   </x:si>
   <x:si>
     <x:t>344122599</x:t>
+  </x:si>
+  <x:si>
+    <x:t>iacopo.depalatis@acpsystem.eu</x:t>
   </x:si>
   <x:si>
     <x:t>GIACOMO</x:t>
@@ -526,7 +532,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:5">
+    <x:row r="1" spans="1:6">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -542,192 +548,228 @@
       <x:c r="E1" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
-    </x:row>
-    <x:row r="3" spans="1:5">
+      <x:c r="F1" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:6">
       <x:c r="A3" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6">
+      <x:c r="A4" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:6">
+      <x:c r="A5" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:6">
+      <x:c r="A6" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:6">
+      <x:c r="A7" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="F7" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:6">
+      <x:c r="A8" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="F8" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:6">
+      <x:c r="A9" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="E3" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:5">
-      <x:c r="A4" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="E4" s="0" t="s">
+      <x:c r="D9" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="F9" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:6">
+      <x:c r="A10" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="F10" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:6">
+      <x:c r="A11" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
-    </x:row>
-    <x:row r="5" spans="1:5">
-      <x:c r="A5" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="C5" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="D5" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="E5" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:5">
-      <x:c r="A6" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="B6" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="C6" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="D6" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="E6" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:5">
-      <x:c r="A7" s="0" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="B7" s="0" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="C7" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="D7" s="0" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="E7" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:5">
-      <x:c r="A8" s="0" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="B8" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="C8" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="D8" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="E8" s="0" t="s">
-        <x:v>31</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:5">
-      <x:c r="A9" s="0" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="B9" s="0" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="C9" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D9" s="0" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="E9" s="0" t="s">
-        <x:v>35</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:5">
-      <x:c r="A10" s="0" t="s">
-        <x:v>36</x:v>
-      </x:c>
-      <x:c r="B10" s="0" t="s">
-        <x:v>37</x:v>
-      </x:c>
-      <x:c r="C10" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="D10" s="0" t="s">
-        <x:v>38</x:v>
-      </x:c>
-      <x:c r="E10" s="0" t="s">
-        <x:v>39</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:5">
-      <x:c r="A11" s="0" t="s">
-        <x:v>40</x:v>
-      </x:c>
-      <x:c r="B11" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="C11" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="E11" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:5">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="F11" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:6">
       <x:c r="A12" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="E12" s="0" t="s">
-        <x:v>47</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:5">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="F12" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:6">
       <x:c r="A13" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="E13" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="F13" s="0" t="s">
+        <x:v>11</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
A few of changes :D
</commit_message>
<xml_diff>
--- a/Output/Candidates.xlsx
+++ b/Output/Candidates.xlsx
@@ -34,136 +34,136 @@
     <x:t>Sender</x:t>
   </x:si>
   <x:si>
+    <x:t>BIAGIO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ROSSI</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FRONTEND DEV</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BIAGIOROSSI@TEST.COM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>321564789</x:t>
+  </x:si>
+  <x:si>
+    <x:t>rafael.casapao@acpsystem.eu</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CARLA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>VERDI</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CARLAVERDI@TEST.COM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>352614789</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PEPPE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PINI</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FULLSTACK DEV</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PEPPEPINI@TEST.COM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>351246897</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CICCIO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BAFO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CICCIOBAFO@TEST.COM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>312589647</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MAX</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MINIMI</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BACKEND DEV</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MAXMINIMI@TEST.COM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>357148623</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PIER</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PIERCUIU</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PIERPIERCUIU@TEST.COM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>364152789</x:t>
+  </x:si>
+  <x:si>
+    <x:t>OLGA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BALEW</x:t>
+  </x:si>
+  <x:si>
+    <x:t>OLGABALEW@TEST.COM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>347158269</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PERLA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DIAMANTI</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PERLADIAMANTI@TEST.COM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>359268147</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GIACOMO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GENSSI</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GIACOMOGESSI@TEST.COM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>349158267</x:t>
+  </x:si>
+  <x:si>
     <x:t>FELE</x:t>
   </x:si>
   <x:si>
     <x:t>BAFELE</x:t>
   </x:si>
   <x:si>
-    <x:t>FRONTEND DEV</x:t>
-  </x:si>
-  <x:si>
     <x:t>FELEBAFELE@TEST.COM</x:t>
   </x:si>
   <x:si>
     <x:t>344122599</x:t>
-  </x:si>
-  <x:si>
-    <x:t>iacopo.depalatis@acpsystem.eu</x:t>
-  </x:si>
-  <x:si>
-    <x:t>GIACOMO</x:t>
-  </x:si>
-  <x:si>
-    <x:t>GENSSI</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BACKEND DEV</x:t>
-  </x:si>
-  <x:si>
-    <x:t>GIACOMOGESSI@TEST.COM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>349158267</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PERLA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DIAMANTI</x:t>
-  </x:si>
-  <x:si>
-    <x:t>FULLSTACK DEV</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PERLADIAMANTI@TEST.COM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>359268147</x:t>
-  </x:si>
-  <x:si>
-    <x:t>OLGA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BALEW</x:t>
-  </x:si>
-  <x:si>
-    <x:t>OLGABALEW@TEST.COM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>347158269</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PIER</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PIERCUIU</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PIERPIERCUIU@TEST.COM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>364152789</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MAX</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MINIMI</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MAXMINIMI@TEST.COM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>357148623</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CICCIO</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BAFO</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CICCIOBAFO@TEST.COM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>312589647</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PEPPE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PINI</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PEPPEPINI@TEST.COM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>351246897</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RICCARDO</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BIANCHI</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RICCARDOBIANCHI@TEST.COM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>369258147</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CARLA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>VERDI</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CARLAVERDI@TEST.COM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>352614789</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -561,40 +561,25 @@
       </x:c>
     </x:row>
     <x:row r="3" spans="1:6">
-      <x:c r="A3" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="E3" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
       <x:c r="F3" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:6">
       <x:c r="A4" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E4" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="F4" s="0" t="s">
         <x:v>11</x:v>
@@ -602,19 +587,19 @@
     </x:row>
     <x:row r="5" spans="1:6">
       <x:c r="A5" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="F5" s="0" t="s">
         <x:v>11</x:v>
@@ -622,19 +607,19 @@
     </x:row>
     <x:row r="6" spans="1:6">
       <x:c r="A6" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="F6" s="0" t="s">
         <x:v>11</x:v>
@@ -642,19 +627,19 @@
     </x:row>
     <x:row r="7" spans="1:6">
       <x:c r="A7" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="E7" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="F7" s="0" t="s">
         <x:v>11</x:v>
@@ -662,19 +647,19 @@
     </x:row>
     <x:row r="8" spans="1:6">
       <x:c r="A8" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="E8" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="F8" s="0" t="s">
         <x:v>11</x:v>
@@ -682,19 +667,19 @@
     </x:row>
     <x:row r="9" spans="1:6">
       <x:c r="A9" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E9" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="F9" s="0" t="s">
         <x:v>11</x:v>
@@ -702,19 +687,19 @@
     </x:row>
     <x:row r="10" spans="1:6">
       <x:c r="A10" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="E10" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="F10" s="0" t="s">
         <x:v>11</x:v>
@@ -722,21 +707,41 @@
     </x:row>
     <x:row r="11" spans="1:6">
       <x:c r="A11" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="E11" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="F11" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:6">
+      <x:c r="A12" s="0" t="s">
         <x:v>46</x:v>
       </x:c>
-      <x:c r="B11" s="0" t="s">
+      <x:c r="B12" s="0" t="s">
         <x:v>47</x:v>
       </x:c>
-      <x:c r="C11" s="0" t="s">
+      <x:c r="C12" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="D11" s="0" t="s">
+      <x:c r="D12" s="0" t="s">
         <x:v>48</x:v>
       </x:c>
-      <x:c r="E11" s="0" t="s">
+      <x:c r="E12" s="0" t="s">
         <x:v>49</x:v>
       </x:c>
-      <x:c r="F11" s="0" t="s">
+      <x:c r="F12" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
Finished Exercise but still to clean
</commit_message>
<xml_diff>
--- a/Output/Candidates.xlsx
+++ b/Output/Candidates.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <x:si>
     <x:t>Name</x:t>
   </x:si>
@@ -34,103 +34,37 @@
     <x:t>Sender</x:t>
   </x:si>
   <x:si>
-    <x:t>CICCIO</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BAFO</x:t>
+    <x:t>FELE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BAFELE</x:t>
   </x:si>
   <x:si>
     <x:t>FRONTEND DEV</x:t>
   </x:si>
   <x:si>
-    <x:t>CICCIOBAFO@TEST.COM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>312589647</x:t>
+    <x:t>FELEBAFELE@TEST.COM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>344122599</x:t>
   </x:si>
   <x:si>
     <x:t>iacopo.depalatis@acpsystem.eu</x:t>
   </x:si>
   <x:si>
-    <x:t>PEPPE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PINI</x:t>
-  </x:si>
-  <x:si>
-    <x:t>FULLSTACK DEV</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PEPPEPINI@TEST.COM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>351246897</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RICCARDO</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BIANCHI</x:t>
+    <x:t>GIACOMO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GENSSI</x:t>
   </x:si>
   <x:si>
     <x:t>BACKEND DEV</x:t>
   </x:si>
   <x:si>
-    <x:t>RICCARDOBIANCHI@TEST.COM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>369258147</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CARLA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>VERDI</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CARLAVERDI@TEST.COM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>352614789</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PIER</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PIERCUIU</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PIERPIERCUIU@TEST.COM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>364152789</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MAX</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MINIMI</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MAXMINIMI@TEST.COM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>357148623</x:t>
-  </x:si>
-  <x:si>
-    <x:t>FELE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BAFELE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>FELEBAFELE@TEST.COM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>344122599</x:t>
-  </x:si>
-  <x:si>
-    <x:t>rafael.casapao@acpsystem.eu</x:t>
+    <x:t>GIACOMOGESSI@TEST.COM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>349158267</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -481,7 +415,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:F11"/>
+  <x:dimension ref="A1:F3"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -545,186 +479,6 @@
       </x:c>
       <x:c r="F3" s="0" t="s">
         <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:6">
-      <x:c r="A4" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="E4" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="F4" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:6">
-      <x:c r="A5" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="C5" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D5" s="0" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="E5" s="0" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="F5" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:6">
-      <x:c r="A6" s="0" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="B6" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="C6" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="D6" s="0" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="E6" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="F6" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:6">
-      <x:c r="A7" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="B7" s="0" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="C7" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="D7" s="0" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="E7" s="0" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="F7" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:6">
-      <x:c r="A8" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="B8" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="C8" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D8" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="E8" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="F8" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:6">
-      <x:c r="A9" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="B9" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="C9" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="D9" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="E9" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="F9" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:6">
-      <x:c r="A10" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="B10" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="C10" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="D10" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="E10" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="F10" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:6">
-      <x:c r="A11" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="B11" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="C11" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D11" s="0" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="E11" s="0" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="F11" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:6">
-      <x:c r="A12" s="0" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="B12" s="0" t="s">
-        <x:v>35</x:v>
-      </x:c>
-      <x:c r="C12" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D12" s="0" t="s">
-        <x:v>36</x:v>
-      </x:c>
-      <x:c r="E12" s="0" t="s">
-        <x:v>37</x:v>
-      </x:c>
-      <x:c r="F12" s="0" t="s">
-        <x:v>38</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>